<commit_message>
Datenstruktur angepasst, Bild davon eingepflegt, Zeitplan wie besprochen angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Datenstruktur_Plattform.xlsx
+++ b/Dokumente/Datenstruktur_Plattform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="2480" windowWidth="28480" windowHeight="20480"/>
+    <workbookView xWindow="2740" yWindow="1780" windowWidth="28480" windowHeight="20480"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,79 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
-  <si>
-    <t>Testarbeitsraum</t>
-  </si>
-  <si>
-    <t>Dokumente</t>
-  </si>
-  <si>
-    <t>Termine</t>
-  </si>
-  <si>
-    <t>Kontakte</t>
-  </si>
-  <si>
-    <t>Hans Muster</t>
-  </si>
-  <si>
-    <t>Maria Meier</t>
-  </si>
-  <si>
-    <t>Adressenblock</t>
-  </si>
-  <si>
-    <t>Auflistungsblock</t>
-  </si>
-  <si>
-    <t>Bild</t>
-  </si>
-  <si>
-    <t>Datei</t>
-  </si>
-  <si>
-    <t>Textblock</t>
-  </si>
-  <si>
-    <t>Merkzettel</t>
-  </si>
-  <si>
-    <t>Kalender</t>
-  </si>
-  <si>
-    <t>.xls</t>
-  </si>
-  <si>
-    <t>.doc</t>
-  </si>
-  <si>
-    <t>.ppt</t>
-  </si>
-  <si>
-    <t>.jpg</t>
-  </si>
-  <si>
-    <t>Startseite</t>
-  </si>
-  <si>
-    <t>Newsportlet</t>
-  </si>
-  <si>
-    <t>News</t>
-  </si>
-  <si>
-    <t>Interne News</t>
-  </si>
-  <si>
-    <t>Beispielnews</t>
-  </si>
-  <si>
-    <t>Arbeitsräume</t>
-  </si>
-  <si>
-    <t>Subsite Teaserportlet</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Ebene1</t>
   </si>
@@ -110,26 +38,128 @@
     <t>Wurzel</t>
   </si>
   <si>
-    <t>Organisation</t>
-  </si>
-  <si>
-    <t>Testtermin</t>
-  </si>
-  <si>
     <t>Ebene5</t>
   </si>
   <si>
-    <t>Traktandum</t>
-  </si>
-  <si>
-    <t>Intranet</t>
+    <t>Aktuell (NewsFolder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Freizeit und Kultur 
+(ContentPage)</t>
+  </si>
+  <si>
+    <t>Regula Meier(Contact)</t>
+  </si>
+  <si>
+    <t>Johann Zbinden(Contact)</t>
+  </si>
+  <si>
+    <t>Ortsplan(Adressenblock)</t>
+  </si>
+  <si>
+    <t>Porträt von Belp(Textblock)</t>
+  </si>
+  <si>
+    <t>600 Jahre Belp(News)</t>
+  </si>
+  <si>
+    <t>Wirtschaft(ContentPage)</t>
+  </si>
+  <si>
+    <t>Projekte(Folder)</t>
+  </si>
+  <si>
+    <t>Gesamtplanung.docx(File)</t>
+  </si>
+  <si>
+    <t>Modell.jpg(File)</t>
+  </si>
+  <si>
+    <t>Kostendach.xlsx(File)</t>
+  </si>
+  <si>
+    <t>Belpberg(Subsite)</t>
+  </si>
+  <si>
+    <t>Porträt(ContentPage)</t>
+  </si>
+  <si>
+    <t>Termine(Events)</t>
+  </si>
+  <si>
+    <t>Tickets(Ticket Box)</t>
+  </si>
+  <si>
+    <t>Flughafenzufahrt Belp
+(Arbeitsraum)</t>
+  </si>
+  <si>
+    <t>Wirtschaftslage von Belp
+(Textblock)</t>
+  </si>
+  <si>
+    <t>GL-Sitzung vom 06.05.2014
+(Meeting)</t>
+  </si>
+  <si>
+    <t>Kostendach überarbeiten
+(Ticket)</t>
+  </si>
+  <si>
+    <t>Gesamtplanung überarbeiten
+(Ticket)</t>
+  </si>
+  <si>
+    <t>Besprechung Kostendach
+(Traktandum)</t>
+  </si>
+  <si>
+    <t>Gemeinde(ContentPage)</t>
+  </si>
+  <si>
+    <t>Politik(ContentPage)</t>
+  </si>
+  <si>
+    <t>Kontakte(Folder)</t>
+  </si>
+  <si>
+    <t>Bilder von Belp
+(Auflistungsblock)</t>
+  </si>
+  <si>
+    <t>Downloads
+(Auflistungsblock)</t>
+  </si>
+  <si>
+    <t>Präsentation 
+Zufahrt.pptx(File)</t>
+  </si>
+  <si>
+    <t>Porträt von Belpberg
+(Textblock)</t>
+  </si>
+  <si>
+    <t>Besprechung 
+Gesamtplanung
+(Traktandum)</t>
+  </si>
+  <si>
+    <t>Belp
+(ContentPage)</t>
+  </si>
+  <si>
+    <t>www.belp.ch
+(PloneSite)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,13 +188,8 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,18 +199,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,18 +216,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -246,8 +265,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -421,22 +490,102 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="217">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -523,6 +672,28 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -609,6 +780,28 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -908,46 +1101,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G32"/>
+  <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="7.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="9.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="12" thickBot="1">
-      <c r="B2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="3" t="s">
-        <v>33</v>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="22">
+      <c r="B3" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -955,297 +1149,333 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" ht="22">
       <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" ht="22">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2"/>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" ht="22">
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="21" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="2"/>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" ht="22">
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="7" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:7" ht="22">
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" ht="22">
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="2"/>
-      <c r="C21" s="4" t="s">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" ht="22">
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" ht="22">
+      <c r="B27" s="2"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" ht="33">
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="G28" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="2:8" ht="33">
+      <c r="B30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:8" ht="33">
+      <c r="B31" s="2"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="G31" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="33">
+      <c r="B32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="G32" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="2"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="5" t="s">
+      <c r="E33" s="4"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="2"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="2"/>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="2"/>
-      <c r="C27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="2:7" ht="22">
+      <c r="B35" s="2"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="2"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ältere Dokumentversionen angeschaut und kontrolliert.
</commit_message>
<xml_diff>
--- a/Dokumente/Datenstruktur_Plattform.xlsx
+++ b/Dokumente/Datenstruktur_Plattform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1780" windowWidth="28480" windowHeight="20480"/>
+    <workbookView xWindow="2740" yWindow="1780" windowWidth="28480" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Ebene1</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Wurzel</t>
-  </si>
-  <si>
-    <t>Ebene5</t>
   </si>
   <si>
     <t>Aktuell (NewsFolder)</t>
@@ -145,10 +142,6 @@
     <t>Besprechung 
 Gesamtplanung
 (Traktandum)</t>
-  </si>
-  <si>
-    <t>Belp
-(ContentPage)</t>
   </si>
   <si>
     <t>www.belp.ch
@@ -189,18 +182,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -535,53 +522,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1101,25 +1085,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="9.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="12" thickBot="1">
+    <row r="2" spans="2:6" ht="12" thickBot="1">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1135,351 +1118,311 @@
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="22">
-      <c r="B3" s="25" t="s">
-        <v>38</v>
+    </row>
+    <row r="3" spans="2:6" ht="33">
+      <c r="B3" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="2:7" ht="22">
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="24" t="s">
-        <v>37</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="C5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="2:7" ht="22">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="2:6" ht="22">
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>8</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:7">
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" ht="22">
+      <c r="C7" s="4"/>
+      <c r="D7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:6" ht="22">
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="E8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="2:6">
       <c r="B9" s="2"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="E9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="2:7" ht="22">
+      <c r="D10" s="4"/>
+      <c r="E10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" ht="22">
       <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="D11" s="4"/>
+      <c r="E11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="C12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:6">
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:7">
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:6">
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:7" ht="22">
+      <c r="D15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:6" ht="22">
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="E16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17" s="2"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18" s="2"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="D18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" s="2"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="D19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:7">
       <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:8" ht="22">
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" ht="22">
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="D21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="2:7">
       <c r="B22" s="2"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:8" ht="22">
+      <c r="E22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" ht="22">
       <c r="B23" s="2"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="E23" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="2:7">
       <c r="B24" s="2"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="E24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="2:7">
       <c r="B25" s="2"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="2:8">
+    </row>
+    <row r="26" spans="2:7">
       <c r="B26" s="2"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="F26" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="2:8" ht="22">
+      <c r="E26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="2:7" ht="22">
       <c r="B27" s="2"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="2:8" ht="33">
+      <c r="E27" s="4"/>
+      <c r="F27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="2:7" ht="33">
       <c r="B28" s="2"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="G28" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="F28" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="2:7">
       <c r="B29" s="2"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="8"/>
+      <c r="D29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="2:8" ht="33">
+    </row>
+    <row r="30" spans="2:7" ht="22">
       <c r="B30" s="2"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="2:8" ht="33">
+      <c r="E30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="2:7" ht="33">
       <c r="B31" s="2"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="G31" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="33">
+      <c r="F31" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="33">
       <c r="B32" s="2"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="G32" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
+      <c r="F32" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
       <c r="B33" s="2"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="6" t="s">
+      <c r="C33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="2"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="2:7" ht="22">
+      <c r="E34" s="9"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="2:6" ht="22">
       <c r="B35" s="2"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:7">
+      <c r="D35" s="2"/>
+      <c r="E35" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="2:6">
       <c r="B36" s="2"/>
-      <c r="C36" s="4"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="2"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Dokument 0.9 abgeschlosen, Bilder hinzugefügt, Zeitplan angepasst..
</commit_message>
<xml_diff>
--- a/Dokumente/Datenstruktur_Plattform.xlsx
+++ b/Dokumente/Datenstruktur_Plattform.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1780" windowWidth="28480" windowHeight="16440"/>
+    <workbookView xWindow="2745" yWindow="1785" windowWidth="28485" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Ebene1</t>
   </si>
@@ -32,120 +32,102 @@
     <t>Ebene3</t>
   </si>
   <si>
-    <t>Ebene4</t>
-  </si>
-  <si>
     <t>Wurzel</t>
   </si>
   <si>
     <t>Aktuell (NewsFolder)</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Freizeit und Kultur 
-(ContentPage)</t>
-  </si>
-  <si>
-    <t>Regula Meier(Contact)</t>
-  </si>
-  <si>
-    <t>Johann Zbinden(Contact)</t>
-  </si>
-  <si>
-    <t>Ortsplan(Adressenblock)</t>
-  </si>
-  <si>
-    <t>Porträt von Belp(Textblock)</t>
-  </si>
-  <si>
-    <t>600 Jahre Belp(News)</t>
-  </si>
-  <si>
-    <t>Wirtschaft(ContentPage)</t>
-  </si>
-  <si>
-    <t>Projekte(Folder)</t>
-  </si>
-  <si>
-    <t>Gesamtplanung.docx(File)</t>
-  </si>
-  <si>
-    <t>Modell.jpg(File)</t>
-  </si>
-  <si>
-    <t>Kostendach.xlsx(File)</t>
-  </si>
-  <si>
     <t>Belpberg(Subsite)</t>
   </si>
   <si>
-    <t>Porträt(ContentPage)</t>
-  </si>
-  <si>
-    <t>Termine(Events)</t>
-  </si>
-  <si>
-    <t>Tickets(Ticket Box)</t>
+    <t>Neues Aktuelles (NewsFolder)</t>
+  </si>
+  <si>
+    <t>Adresse (AddressBlock)</t>
+  </si>
+  <si>
+    <t>gemeinde
+(PloneSite)</t>
+  </si>
+  <si>
+    <t>Abwasserreglement (News)</t>
+  </si>
+  <si>
+    <t>Kulturtage (News)</t>
+  </si>
+  <si>
+    <t>Jugend (ContentPage)</t>
+  </si>
+  <si>
+    <t>Paragraph1 (TextBlock)</t>
+  </si>
+  <si>
+    <t>Bilder (ListingBlock)</t>
+  </si>
+  <si>
+    <t>image1 (Image)</t>
+  </si>
+  <si>
+    <t>image2 (Image)</t>
+  </si>
+  <si>
+    <t>image3 (Image)</t>
+  </si>
+  <si>
+    <t>Zusammenarbeit (TextBlock)</t>
+  </si>
+  <si>
+    <t>Prix Belp (TextBlock)</t>
+  </si>
+  <si>
+    <t>Kräfteverhältnis (TextBlock)</t>
+  </si>
+  <si>
+    <t>600 Jahre Belp (News)</t>
+  </si>
+  <si>
+    <t>Kontakte (Folder)</t>
+  </si>
+  <si>
+    <t>Projekte (Folder)</t>
   </si>
   <si>
     <t>Flughafenzufahrt Belp
-(Arbeitsraum)</t>
-  </si>
-  <si>
-    <t>Wirtschaftslage von Belp
-(Textblock)</t>
-  </si>
-  <si>
-    <t>GL-Sitzung vom 06.05.2014
-(Meeting)</t>
-  </si>
-  <si>
-    <t>Kostendach überarbeiten
-(Ticket)</t>
-  </si>
-  <si>
-    <t>Gesamtplanung überarbeiten
-(Ticket)</t>
-  </si>
-  <si>
-    <t>Besprechung Kostendach
-(Traktandum)</t>
-  </si>
-  <si>
-    <t>Gemeinde(ContentPage)</t>
-  </si>
-  <si>
-    <t>Politik(ContentPage)</t>
-  </si>
-  <si>
-    <t>Kontakte(Folder)</t>
-  </si>
-  <si>
-    <t>Bilder von Belp
-(Auflistungsblock)</t>
-  </si>
-  <si>
-    <t>Downloads
-(Auflistungsblock)</t>
-  </si>
-  <si>
-    <t>Präsentation 
-Zufahrt.pptx(File)</t>
-  </si>
-  <si>
-    <t>Porträt von Belpberg
-(Textblock)</t>
-  </si>
-  <si>
-    <t>Besprechung 
-Gesamtplanung
-(Traktandum)</t>
-  </si>
-  <si>
-    <t>www.belp.ch
-(PloneSite)</t>
+(Workspace)</t>
+  </si>
+  <si>
+    <t>Flughafen (Image)</t>
+  </si>
+  <si>
+    <t>Evaluation.xlsx (File)</t>
+  </si>
+  <si>
+    <t>IT.docx (File)</t>
+  </si>
+  <si>
+    <t>Nachhaltigkeit.pdf (File)</t>
+  </si>
+  <si>
+    <t>Porträt (ContentPage)</t>
+  </si>
+  <si>
+    <t>Intro (Textblock)</t>
+  </si>
+  <si>
+    <t>Bild (Image)</t>
+  </si>
+  <si>
+    <t>Lebensqualität (ContentPage)</t>
+  </si>
+  <si>
+    <t>Verwaltung (ContentPage)</t>
+  </si>
+  <si>
+    <t>Wirtschaft Gewerbe (ContentPage)</t>
+  </si>
+  <si>
+    <t>Politik (ContentPage)</t>
   </si>
 </sst>
 </file>
@@ -182,7 +164,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,12 +185,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -220,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -275,31 +251,58 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -522,162 +525,147 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="217">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -786,7 +774,7 @@
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1085,26 +1073,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G36"/>
+  <dimension ref="B2:E35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="12" thickBot="1">
+    <row r="2" spans="2:5" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -1112,317 +1099,277 @@
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="33">
-      <c r="B3" s="24" t="s">
-        <v>36</v>
+    </row>
+    <row r="3" spans="2:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="2"/>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" ht="22">
-      <c r="B6" s="2"/>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="2"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:6" ht="22">
-      <c r="B8" s="2"/>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="10"/>
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="2"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" ht="22">
-      <c r="B11" s="2"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+      <c r="C12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="2"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="10"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="10"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="2"/>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="10"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" ht="22">
-      <c r="B16" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="10"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="2"/>
-      <c r="C17" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="E16" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="10"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="2"/>
+      <c r="E17" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="10"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="2"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="2"/>
-      <c r="C20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" ht="22">
-      <c r="B21" s="2"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="10"/>
+      <c r="C19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="10"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="10"/>
+      <c r="C21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="10"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:7" ht="22">
-      <c r="B23" s="2"/>
+      <c r="D22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="2"/>
+      <c r="D23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="10"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="2"/>
-      <c r="C25" s="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="10"/>
+      <c r="C25" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="E26" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="2:7" ht="22">
-      <c r="B27" s="2"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="10"/>
+      <c r="C26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="2:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="B27" s="10"/>
       <c r="C27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="19" t="s">
+      <c r="D27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="10"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="10"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="2:7" ht="33">
-      <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="F28" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="2"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="2:7" ht="22">
-      <c r="B30" s="2"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="10"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="2:7" ht="33">
-      <c r="B31" s="2"/>
+      <c r="E30" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="10"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="F31" s="19" t="s">
+      <c r="E31" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="33">
-      <c r="B32" s="2"/>
-      <c r="C32" s="4"/>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="7"/>
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D32" s="4"/>
-      <c r="F32" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="2"/>
-      <c r="C33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="2:6" ht="22">
-      <c r="B35" s="2"/>
-      <c r="C35" s="4"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="7"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="7"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="7"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="2"/>
+      <c r="E35" s="17" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1437,7 +1384,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1454,7 +1401,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>